<commit_message>
Cleaning up Fig 1 length.
</commit_message>
<xml_diff>
--- a/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
+++ b/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/4 Reviewer Comments 1 and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3C9B24-B232-124B-AB37-AE5E322DD2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BBF1A4-327C-7341-B87F-35ED3BD91E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38240" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -66,9 +66,6 @@
     <t>consider adding relevant referemces from the same Publisher as I cannot trace back any. As an example, you may refer to "G. Evola, V. Costanzo, L. Marletta, Exergy analysis of energy systems in buildings, Buildings 8 (2018), 180"</t>
   </si>
   <si>
-    <t xml:space="preserve">The manuscript was prepared with the LaTeX template provided by MDPI. Thus, the manuscript should be very close to consistent already. That said, we reviewed the requirements at https://www.mdpi.com/journal/energies/instructions to ensure compliance. </t>
-  </si>
-  <si>
     <t>Review https://www.mdpi.com/journal/energies/instructions and make any changes deemed necessary.</t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>Responses to Round 2 comments (academic editor comments)</t>
+  </si>
+  <si>
+    <t>The manuscript was prepared with the LaTeX template provided by MDPI. Thus, the manuscript should be very close to consistent already. That said, we reviewed the requirements at https://www.mdpi.com/journal/energies/instructions. To the best of our knowledge, we are in compliance with the formatting of the journal template.</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -137,12 +140,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -167,9 +176,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -182,6 +188,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,7 +1707,7 @@
   <dimension ref="A3:AMK14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,7 +1733,7 @@
     </row>
     <row r="5" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1025" ht="24" x14ac:dyDescent="0.3">
@@ -1743,23 +1758,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
+    <row r="11" spans="1:1025" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
+      <c r="F11" s="12" t="s">
+        <v>23</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -2780,21 +2797,21 @@
       <c r="AMJ11" s="5"/>
       <c r="AMK11" s="5"/>
     </row>
-    <row r="12" spans="1:1025" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1025" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>15</v>
+      <c r="E12" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3815,21 +3832,21 @@
       <c r="AMJ12" s="4"/>
       <c r="AMK12" s="4"/>
     </row>
-    <row r="13" spans="1:1025" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1025" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>16</v>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -4850,21 +4867,21 @@
       <c r="AMJ13" s="4"/>
       <c r="AMK13" s="4"/>
     </row>
-    <row r="14" spans="1:1025" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1025" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>17</v>
+      <c r="E14" s="8" t="s">
+        <v>16</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>

</xml_diff>

<commit_message>
Moved Fig 1 caption text out of the caption
</commit_message>
<xml_diff>
--- a/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
+++ b/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/4 Reviewer Comments 1 and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BBF1A4-327C-7341-B87F-35ED3BD91E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0D9344-7A43-7843-BE8F-B3BAB4EB087B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38240" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>We moved mjuch of the text of the Fig. 1 caption to two places in the paper: just after the figure and to section 2.2.2 where lamps and the LSPDD are discussed.</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1710,7 @@
   <dimension ref="A3:AMK14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2797,14 +2800,16 @@
       <c r="AMJ11" s="5"/>
       <c r="AMK11" s="5"/>
     </row>
-    <row r="12" spans="1:1025" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1025" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="8" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Movig text from Figure 2.
</commit_message>
<xml_diff>
--- a/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
+++ b/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/4 Reviewer Comments 1 and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0D9344-7A43-7843-BE8F-B3BAB4EB087B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4DE3EC-EBBB-394D-8048-BFE78440B574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38240" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,13 +93,13 @@
     <t>Responses to Round 2 comments (academic editor comments)</t>
   </si>
   <si>
-    <t>The manuscript was prepared with the LaTeX template provided by MDPI. Thus, the manuscript should be very close to consistent already. That said, we reviewed the requirements at https://www.mdpi.com/journal/energies/instructions. To the best of our knowledge, we are in compliance with the formatting of the journal template.</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
     <t>We moved mjuch of the text of the Fig. 1 caption to two places in the paper: just after the figure and to section 2.2.2 where lamps and the LSPDD are discussed.</t>
+  </si>
+  <si>
+    <t>The manuscript was prepared with the LaTeX template provided by MDPI. Thus, the manuscript should be very close to consistent already. That said, we reviewed the requirements at https://www.mdpi.com/journal/energies/instructions. We found one case where we were not in compliance with the journal's formatting requirements, wpecifically, we typeset page references as "[17, p. 152]", but they should be "[17] (p. 152)". We fixed all of these page references to comply with the journal's specifications.</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1710,7 @@
   <dimension ref="A3:AMK14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1761,7 +1761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1025" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>7</v>
@@ -1778,7 +1778,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2808,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Move tables from appendix.
</commit_message>
<xml_diff>
--- a/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
+++ b/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/4 Reviewer Comments 1 and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E437E286-396B-DA4E-B950-466A4D291051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E377D687-09F9-4949-99F2-1E9628CD32D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38240" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>We moved much of the text of the Fig. 1 caption to two places in the paper: just after the figure and to section 2.2.2 where lamps and the LSPDD are discussed. Text from the Fig. 2 caption was moved to the paragraph in which we refer to Figure 2.</t>
+  </si>
+  <si>
+    <t>We interpreted this comment as "remove Tables A1 and A2 from the appendix," which we have done. The tables are now incorporated into the body of the paper. With this change, the appendix has been eliminated from the paper. We think this is a positivie change, as the backmatter is streamlined compared to our previous submission. Thanks!</t>
   </si>
 </sst>
 </file>
@@ -1709,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3839,21 +3842,25 @@
       <c r="AMJ12" s="4"/>
       <c r="AMK12" s="4"/>
     </row>
-    <row r="13" spans="1:1025" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:1025" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>

</xml_diff>

<commit_message>
Respond to "more references" comment.
</commit_message>
<xml_diff>
--- a/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
+++ b/Submissions/4 Reviewer Comments 1 and Response/Lighting Paper Acad Editor Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/4 Reviewer Comments 1 and Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E377D687-09F9-4949-99F2-1E9628CD32D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3E6B24-97AA-FB42-8171-C48D4BFCB17B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38240" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>The Energy and Exergy of Light</t>
   </si>
@@ -104,12 +104,37 @@
   <si>
     <t>We interpreted this comment as "remove Tables A1 and A2 from the appendix," which we have done. The tables are now incorporated into the body of the paper. With this change, the appendix has been eliminated from the paper. We think this is a positivie change, as the backmatter is streamlined compared to our previous submission. Thanks!</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We added 7 new references, 4 of which are in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Energies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -145,6 +170,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -172,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,14 +215,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1712,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,23 +1790,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:1025" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="5"/>
@@ -2803,23 +2829,23 @@
       <c r="AMJ11" s="5"/>
       <c r="AMK11" s="5"/>
     </row>
-    <row r="12" spans="1:1025" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:1025" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="4"/>
@@ -3842,23 +3868,23 @@
       <c r="AMJ12" s="4"/>
       <c r="AMK12" s="4"/>
     </row>
-    <row r="13" spans="1:1025" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:1025" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="4"/>
@@ -4881,21 +4907,25 @@
       <c r="AMJ13" s="4"/>
       <c r="AMK13" s="4"/>
     </row>
-    <row r="14" spans="1:1025" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:1025" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>

</xml_diff>